<commit_message>
Final version for essay
</commit_message>
<xml_diff>
--- a/data/ipo_db.xlsx
+++ b/data/ipo_db.xlsx
@@ -5,24 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramu/IPO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramu/B2B_SaaS_IPO_Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4621C8BF-E994-8C4D-B726-07F363553F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF683611-DC34-D340-A104-A33DBDB5AF09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1640" windowWidth="26440" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="1640" windowWidth="26440" windowHeight="14120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipo_db" sheetId="1" r:id="rId1"/>
-    <sheet name="FSLY" sheetId="3" r:id="rId2"/>
-    <sheet name="WK" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="NET" sheetId="8" r:id="rId3"/>
+    <sheet name="ZM" sheetId="6" r:id="rId4"/>
+    <sheet name="ESTC" sheetId="7" r:id="rId5"/>
+    <sheet name="DDOG" sheetId="5" r:id="rId6"/>
+    <sheet name="FSLY" sheetId="3" r:id="rId7"/>
+    <sheet name="WK" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="166">
   <si>
     <t>ticker</t>
   </si>
@@ -481,6 +486,45 @@
   </si>
   <si>
     <t>ignore</t>
+  </si>
+  <si>
+    <t>Customers &gt; $100K</t>
+  </si>
+  <si>
+    <t>Revenue % from enterprise customers</t>
+  </si>
+  <si>
+    <t>Total customers</t>
+  </si>
+  <si>
+    <t>Customers &gt; $1M</t>
+  </si>
+  <si>
+    <t>Customer concentration</t>
+  </si>
+  <si>
+    <t>As of June 30, 2019, our 10 largest customers represented approximately 14% of our ARR and no single customer represented more than 5% of our ARR</t>
+  </si>
+  <si>
+    <t>Customers &gt;= $100K</t>
+  </si>
+  <si>
+    <t>Customers &gt;= $100K (% Revenue)</t>
+  </si>
+  <si>
+    <t>Customers &gt;= $1M</t>
+  </si>
+  <si>
+    <t>Customers &gt;= $1M (% Revenue)</t>
+  </si>
+  <si>
+    <t>Funding</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Total Funding</t>
   </si>
 </sst>
 </file>
@@ -968,11 +1012,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1331,11 +1377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6265,6 +6311,863 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052AA35D-B646-BC40-A06B-0B248EB4D7A4}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>590</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="F2">
+        <v>8800</v>
+      </c>
+      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98483EE-0C73-2F4D-9DCB-6CDC0F95AF5B}">
+  <dimension ref="B1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>40118</v>
+      </c>
+      <c r="G2">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>40725</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5">
+        <f>G3/SUM(G2:G3)</f>
+        <v>0.90702947845804982</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>41609</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5">
+        <f>G4/SUM(G2:G4)</f>
+        <v>0.69396252602359476</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>42248</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="G5">
+        <v>110</v>
+      </c>
+      <c r="H5" s="3">
+        <f>G5/SUM(G2:G5)</f>
+        <v>0.60422960725075525</v>
+      </c>
+      <c r="J5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5">
+        <f>SUM(G2:G11)</f>
+        <v>332.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>42735</v>
+      </c>
+      <c r="C6">
+        <v>95</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>43100</v>
+      </c>
+      <c r="C7">
+        <v>184</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>43281</v>
+      </c>
+      <c r="C8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>43465</v>
+      </c>
+      <c r="C9">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>43525</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="G10">
+        <v>150</v>
+      </c>
+      <c r="H10" s="5">
+        <f>G10/SUM(G2:G10)</f>
+        <v>0.45173919590423128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>43646</v>
+      </c>
+      <c r="C11">
+        <v>408</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B2:G11">
+    <sortCondition ref="B2:B11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72671E1-5528-A041-B26D-60D235DA9DAA}">
+  <dimension ref="B1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>40210</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>40695</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>41275</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>41518</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>42036</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>42736</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <f>SUM(G2:G7)</f>
+        <v>146</v>
+      </c>
+      <c r="J7" s="3">
+        <f>G7/I7</f>
+        <v>0.68493150684931503</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>42766</v>
+      </c>
+      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>43131</v>
+      </c>
+      <c r="C9">
+        <v>143</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>43496</v>
+      </c>
+      <c r="C10">
+        <v>344</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B2:G10">
+    <sortCondition ref="B2:B10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D7E48A-8033-B34E-9E0C-780D744E2223}">
+  <dimension ref="B1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>41214</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>41306</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="G3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>41791</v>
+      </c>
+      <c r="G4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>42552</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>42855</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>43220</v>
+      </c>
+      <c r="C7">
+        <v>275</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="I7">
+        <f>SUM(G2:G5)</f>
+        <v>162</v>
+      </c>
+      <c r="J7" s="3">
+        <f>G5/I7</f>
+        <v>0.35802469135802467</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>43312</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="D9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B2:G9">
+    <sortCondition ref="B2:B9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF62C3E-EC83-2E4E-B2E6-2944067B840D}">
+  <dimension ref="B1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>40634</v>
+      </c>
+      <c r="G2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>41214</v>
+      </c>
+      <c r="G3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>41671</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>42005</v>
+      </c>
+      <c r="G5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G6">
+        <v>94.5</v>
+      </c>
+      <c r="I6">
+        <f>SUM(G2:G6)</f>
+        <v>147.9</v>
+      </c>
+      <c r="J6" s="3">
+        <f>G6/I6</f>
+        <v>0.63894523326572006</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>42735</v>
+      </c>
+      <c r="C7">
+        <v>130</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>43100</v>
+      </c>
+      <c r="C8">
+        <v>240</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>43465</v>
+      </c>
+      <c r="C9">
+        <v>450</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>43646</v>
+      </c>
+      <c r="C10">
+        <v>590</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="E10">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B2:H12">
+    <sortCondition ref="B2:B12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D6:N19"/>
   <sheetViews>
@@ -6539,7 +7442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D4:N17"/>
   <sheetViews>

</xml_diff>